<commit_message>
Inclusao dos ultimos resultados ate 09/09/2017
</commit_message>
<xml_diff>
--- a/ultimosjogos.xlsx
+++ b/ultimosjogos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
   <si>
     <t>SIM</t>
   </si>
@@ -32,12 +32,18 @@
   <si>
     <t>NÃO</t>
   </si>
+  <si>
+    <t>JARDIM</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -67,8 +73,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -79,6 +91,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9E6F4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E6F4"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -96,7 +114,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -114,6 +132,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -449,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1026,29 +1062,134 @@
         <v>53199978.32</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
-      <c r="C10" s="4">
+    <row r="10" spans="1:21" ht="24">
+      <c r="A10" s="7">
+        <v>1965</v>
+      </c>
+      <c r="B10" s="8">
+        <v>42984</v>
+      </c>
+      <c r="C10" s="7">
+        <v>28</v>
+      </c>
+      <c r="D10" s="7">
         <v>26</v>
       </c>
-      <c r="D10" s="4">
-        <v>28</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="E10" s="7">
+        <v>55</v>
+      </c>
+      <c r="F10" s="7">
+        <v>38</v>
+      </c>
+      <c r="G10" s="7">
+        <v>48</v>
+      </c>
+      <c r="H10" s="7">
         <v>35</v>
       </c>
-      <c r="F10" s="4">
-        <v>38</v>
-      </c>
-      <c r="G10" s="4">
-        <v>48</v>
-      </c>
-      <c r="H10" s="4">
-        <v>55</v>
+      <c r="I10" s="9">
+        <v>79933521.5</v>
+      </c>
+      <c r="J10" s="7">
+        <v>1</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M10" s="7">
+        <v>78022245.310000002</v>
+      </c>
+      <c r="N10" s="7">
+        <v>98</v>
+      </c>
+      <c r="O10" s="9">
+        <v>47025.82</v>
+      </c>
+      <c r="P10" s="7">
+        <v>6377</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>1032.4000000000001</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="S10" s="9">
+        <v>0</v>
+      </c>
+      <c r="T10" s="9">
+        <v>2500000</v>
+      </c>
+      <c r="U10" s="9">
+        <v>54412749.609999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="10">
+        <v>1966</v>
+      </c>
+      <c r="B11" s="11">
+        <v>42987</v>
+      </c>
+      <c r="C11" s="10">
+        <v>19</v>
+      </c>
+      <c r="D11" s="10">
+        <v>10</v>
+      </c>
+      <c r="E11" s="10">
+        <v>32</v>
+      </c>
+      <c r="F11" s="10">
+        <v>60</v>
+      </c>
+      <c r="G11" s="10">
+        <v>13</v>
+      </c>
+      <c r="H11" s="10">
+        <v>40</v>
+      </c>
+      <c r="I11" s="12">
+        <v>23689603</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0</v>
+      </c>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10">
+        <v>0</v>
+      </c>
+      <c r="N11" s="10">
+        <v>29</v>
+      </c>
+      <c r="O11" s="12">
+        <v>47097.01</v>
+      </c>
+      <c r="P11" s="10">
+        <v>2758</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>707.45</v>
+      </c>
+      <c r="R11" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" s="12">
+        <v>2515971.84</v>
+      </c>
+      <c r="T11" s="12">
+        <v>5500000</v>
+      </c>
+      <c r="U11" s="12">
+        <v>54772174.170000002</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>